<commit_message>
4oct-codigo pronto checklist pronta
</commit_message>
<xml_diff>
--- a/tablaPrecarga.xlsx
+++ b/tablaPrecarga.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5dcd86d9bf03d87f/ORT/Semestre2/P2/Obligatorio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="246" documentId="8_{382E993F-35F1-4BF2-A315-7D97484DF210}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5867C0ED-1F40-4F0E-A93B-77E436F4A287}"/>
+  <xr:revisionPtr revIDLastSave="250" documentId="8_{382E993F-35F1-4BF2-A315-7D97484DF210}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5532811D-DD82-4681-A143-A680909C4141}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="1" xr2:uid="{1C8C28BD-6758-41E3-A33B-63D4B3187785}"/>
   </bookViews>
@@ -215,7 +215,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -230,6 +230,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -826,7 +829,7 @@
   <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -849,30 +852,30 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="2">
+      <c r="B2" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="6">
         <v>30</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="6">
         <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="2">
+      <c r="B3" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="6">
         <v>50</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="6">
         <v>130</v>
       </c>
     </row>
@@ -892,422 +895,422 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="4">
-        <v>25</v>
-      </c>
-      <c r="D5" s="4">
-        <v>289</v>
+        <v>37</v>
+      </c>
+      <c r="C5" s="2">
+        <v>50</v>
+      </c>
+      <c r="D5" s="2">
+        <v>542</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" s="4">
-        <v>49</v>
-      </c>
-      <c r="D6" s="4">
-        <v>304</v>
+      <c r="A6" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="6">
+        <v>87</v>
+      </c>
+      <c r="D6" s="6">
+        <v>614</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="3">
+        <v>30</v>
+      </c>
+      <c r="D7" s="3">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" s="5">
-        <v>70</v>
-      </c>
-      <c r="D7" s="5">
-        <v>728</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>38</v>
+      <c r="B8" s="6" t="s">
+        <v>39</v>
       </c>
       <c r="C8" s="4">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="D8" s="4">
-        <v>297</v>
+        <v>289</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C9" s="4">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="D9" s="4">
-        <v>105</v>
+        <v>304</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>37</v>
       </c>
       <c r="C10" s="5">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="D10" s="5">
-        <v>111</v>
+        <v>728</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="4" t="s">
+      <c r="A11" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="4">
-        <v>60</v>
-      </c>
-      <c r="D11" s="4">
-        <v>716</v>
+      <c r="C11" s="6">
+        <v>89</v>
+      </c>
+      <c r="D11" s="6">
+        <v>388</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="4">
-        <v>75</v>
-      </c>
-      <c r="D12" s="4">
-        <v>732</v>
+        <v>25</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="2">
+        <v>15</v>
+      </c>
+      <c r="D12" s="2">
+        <v>494</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" s="5">
-        <v>80</v>
-      </c>
-      <c r="D13" s="5">
-        <v>728</v>
+        <v>25</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="3">
+        <v>49</v>
+      </c>
+      <c r="D13" s="3">
+        <v>497</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="4">
+        <v>20</v>
+      </c>
+      <c r="D14" s="4">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="4">
+        <v>80</v>
+      </c>
+      <c r="D15" s="4">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="2">
-        <v>10</v>
-      </c>
-      <c r="D14" s="2">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="2">
-        <v>50</v>
-      </c>
-      <c r="D15" s="2">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" s="2">
-        <v>60</v>
-      </c>
-      <c r="D16" s="2">
-        <v>129</v>
+      <c r="C16" s="5">
+        <v>15</v>
+      </c>
+      <c r="D16" s="5">
+        <v>297</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" s="3">
-        <v>85</v>
-      </c>
-      <c r="D17" s="3">
-        <v>735</v>
+      <c r="A17" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="6">
+        <v>88</v>
+      </c>
+      <c r="D17" s="6">
+        <v>490</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" s="2" t="s">
+      <c r="A18" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="2">
-        <v>32</v>
-      </c>
-      <c r="D18" s="2">
-        <v>238</v>
+      <c r="C18" s="6">
+        <v>53</v>
+      </c>
+      <c r="D18" s="6">
+        <v>498</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="3" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C19" s="3">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="D19" s="3">
-        <v>307</v>
+        <v>598</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" s="2">
-        <v>50</v>
-      </c>
-      <c r="D20" s="2">
-        <v>542</v>
+        <v>18</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="4">
+        <v>60</v>
+      </c>
+      <c r="D20" s="4">
+        <v>716</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" s="2">
-        <v>87</v>
-      </c>
-      <c r="D21" s="2">
-        <v>614</v>
+      <c r="A21" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="4">
+        <v>80</v>
+      </c>
+      <c r="D21" s="4">
+        <v>728</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C22" s="3">
-        <v>30</v>
-      </c>
-      <c r="D22" s="3">
-        <v>617</v>
+        <v>18</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="5">
+        <v>75</v>
+      </c>
+      <c r="D22" s="5">
+        <v>732</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C23" s="2">
-        <v>89</v>
+        <v>20</v>
       </c>
       <c r="D23" s="2">
-        <v>388</v>
+        <v>393</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C24" s="2">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="D24" s="2">
-        <v>494</v>
+        <v>396</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="3" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>37</v>
       </c>
       <c r="C25" s="3">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="D25" s="3">
-        <v>497</v>
+        <v>396</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="2" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>38</v>
       </c>
       <c r="C26" s="2">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D26" s="2">
-        <v>598</v>
+        <v>110</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="2" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C27" s="2">
-        <v>88</v>
+        <v>50</v>
       </c>
       <c r="D27" s="2">
-        <v>490</v>
+        <v>129</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="3" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B28" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" s="3">
+        <v>60</v>
+      </c>
+      <c r="D28" s="3">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="6">
+        <v>85</v>
+      </c>
+      <c r="D29" s="6">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C28" s="3">
-        <v>53</v>
-      </c>
-      <c r="D28" s="3">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C29" s="2">
-        <v>20</v>
-      </c>
-      <c r="D29" s="2">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C30" s="2">
-        <v>40</v>
-      </c>
-      <c r="D30" s="2">
-        <v>396</v>
+      <c r="C30" s="6">
+        <v>23</v>
+      </c>
+      <c r="D30" s="6">
+        <v>375</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C31" s="3">
-        <v>53</v>
+        <v>88</v>
       </c>
       <c r="D31" s="3">
-        <v>396</v>
+        <v>378</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="2" t="s">
+      <c r="A32" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C32" s="2">
-        <v>23</v>
-      </c>
-      <c r="D32" s="2">
-        <v>375</v>
+      <c r="B32" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" s="6">
+        <v>34</v>
+      </c>
+      <c r="D32" s="6">
+        <v>611</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="2" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>38</v>
       </c>
       <c r="C33" s="2">
-        <v>88</v>
+        <v>32</v>
       </c>
       <c r="D33" s="2">
-        <v>378</v>
+        <v>238</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="3" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C34" s="3">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="D34" s="3">
-        <v>611</v>
+        <v>307</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -1353,30 +1356,30 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" s="2" t="s">
+      <c r="A38" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C38" s="2">
-        <v>60</v>
-      </c>
-      <c r="D38" s="2">
-        <v>506</v>
+      <c r="B38" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C38" s="6">
+        <v>75</v>
+      </c>
+      <c r="D38" s="6">
+        <v>501</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" s="2" t="s">
+      <c r="A39" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C39" s="2">
-        <v>75</v>
-      </c>
-      <c r="D39" s="2">
+      <c r="B39" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C39" s="6">
+        <v>80</v>
+      </c>
+      <c r="D39" s="6">
         <v>501</v>
       </c>
     </row>
@@ -1385,13 +1388,13 @@
         <v>33</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C40" s="3">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="D40" s="3">
-        <v>501</v>
+        <v>506</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -1402,10 +1405,10 @@
         <v>37</v>
       </c>
       <c r="C41" s="2">
-        <v>30</v>
+        <v>64</v>
       </c>
       <c r="D41" s="2">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -1416,10 +1419,10 @@
         <v>37</v>
       </c>
       <c r="C42" s="2">
-        <v>64</v>
+        <v>30</v>
       </c>
       <c r="D42" s="2">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -1437,6 +1440,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D43">
+    <sortCondition ref="A2:A43"/>
+  </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>